<commit_message>
update data file with Git repo metadata
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_1.xlsx
+++ b/tests/fixtures/data_file_1.xlsx
@@ -1,21 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/migration_test_repo/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1400" yWindow="6440" windowWidth="19180" windowHeight="11180"/>
+    <workbookView xWindow="-18400" yWindow="7000" windowWidth="17640" windowHeight="8820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Git metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Tests" sheetId="2" r:id="rId2"/>
-    <sheet name="References" sheetId="3" r:id="rId3"/>
+    <sheet name="Data repo metadata" sheetId="5" r:id="rId1"/>
+    <sheet name="Schema repo metadata" sheetId="4" r:id="rId2"/>
+    <sheet name="Tests" sheetId="2" r:id="rId3"/>
+    <sheet name="References" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">References!$A$1:$B$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">References!$A$1:$B$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tests!$A$1:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -86,50 +101,36 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long
-Enter a string.
-Value must be between 1 and 63 characters.
-Value must be unique.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter an integer.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a comma-separated list of values from "References:A" or blank.</t>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
         </r>
       </text>
     </comment>
@@ -168,6 +169,72 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter an integer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a comma-separated list of values from "References:A" or blank.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long
+Enter a string.
+Value must be between 1 and 63 characters.
+Value must be unique.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Enter a Boolean value
 Select "True" or "False".</t>
         </r>
@@ -178,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Url</t>
   </si>
@@ -231,8 +298,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,13 +315,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -286,9 +353,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -302,6 +368,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -348,12 +419,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -380,14 +451,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -414,6 +486,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,54 +662,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="3">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B1">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
@@ -646,45 +721,107 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <dataValidations count="3">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B1">
+      <formula1>255</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -692,11 +829,11 @@
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:D2"/>
   <dataValidations count="4">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="A2">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." sqref="A2">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
       <formula1>255</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Existing attr" error="Value must be an integer." promptTitle="Existing attr" prompt="Enter an integer." sqref="C2">
@@ -710,42 +847,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="b">
+      <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="b">
+      <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -753,11 +891,11 @@
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:B3"/>
   <dataValidations count="2">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="A2:A3">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." sqref="A2:A3">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Published" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Published" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="B2:B3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Published" error="Enter a Boolean value_x000a__x000a_Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Published" prompt="Enter a Boolean value_x000a__x000a_Select &quot;True&quot; or &quot;False&quot;." sqref="B2:B3">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updating for changes to ObjTables
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_1.xlsx
+++ b/tests/fixtures/data_file_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" activeTab="3"/>
+    <workbookView windowWidth="20295" windowHeight="6840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="!Data repo metadata" sheetId="5" r:id="rId1"/>
@@ -221,7 +221,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='DataRepoMetadata' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='DataRepoMetadata' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Branch</t>
@@ -242,10 +242,10 @@
     <t>https://github.com/KarrLab/migration_test_repo.git</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='SchemaRepoMetadata' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables TableType='Data' ModelId='Test' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='SchemaRepoMetadata' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='Test' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Id</t>
@@ -269,7 +269,7 @@
     <t>ref_1, ref_2</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Reference' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Reference' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Published</t>
@@ -286,12 +286,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,23 +307,70 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,12 +383,48 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -350,10 +433,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -364,112 +456,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -492,187 +478,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,56 +669,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -755,7 +691,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -777,157 +728,192 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -936,14 +922,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>

</xml_diff>

<commit_message>
updating fixtures for obj_tables
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_1.xlsx
+++ b/tests/fixtures/data_file_1.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6840" activeTab="3"/>
+    <workbookView windowWidth="28695" windowHeight="14070" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="!Data repo metadata" sheetId="5" r:id="rId1"/>
-    <sheet name="!Schema repo metadata" sheetId="4" r:id="rId2"/>
-    <sheet name="!Tests" sheetId="2" r:id="rId3"/>
-    <sheet name="!References" sheetId="3" r:id="rId4"/>
+    <sheet name="!!Data repo metadata" sheetId="5" r:id="rId1"/>
+    <sheet name="!!Schema repo metadata" sheetId="4" r:id="rId2"/>
+    <sheet name="!!Tests" sheetId="2" r:id="rId3"/>
+    <sheet name="!!References" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!Tests'!$A$2:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!References'!$A$2:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Tests'!$A$2:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!!References'!$A$2:$B$4</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -286,10 +286,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -313,6 +313,96 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -322,22 +412,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,104 +433,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -456,6 +440,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -478,115 +478,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,67 +658,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,30 +669,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -707,6 +683,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -737,21 +746,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -761,159 +755,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
updating for changes to formatting of document, table metadata
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_1.xlsx
+++ b/tests/fixtures/data_file_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" activeTab="3"/>
+    <workbookView windowWidth="19800" windowHeight="5850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="!!Data repo metadata" sheetId="5" r:id="rId1"/>
@@ -221,7 +221,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
-    <t>!!ObjTables Type='Data' Id='DataRepoMetadata' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' id='DataRepoMetadata' date='2019-09-18 13:17:59' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Branch</t>
@@ -242,10 +242,10 @@
     <t>https://github.com/KarrLab/migration_test_repo.git</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='SchemaRepoMetadata' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Data' Id='Test' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' id='SchemaRepoMetadata' date='2019-09-18 13:17:59' objTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' id='Test' date='2019-09-18 13:17:59' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Id</t>
@@ -269,7 +269,7 @@
     <t>ref_1, ref_2</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Reference' Date='2019-09-18 13:17:59' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' id='Reference' date='2019-09-18 13:17:59' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Published</t>
@@ -286,12 +286,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +313,118 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -321,107 +433,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -433,28 +457,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <name val="Tahoma"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -478,19 +483,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,163 +651,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,6 +674,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -683,24 +697,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -746,15 +742,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -769,151 +756,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -999,10 +1004,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="212121"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F3F3F3"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>

</xml_diff>